<commit_message>
phase 1 working, balance log exports too
</commit_message>
<xml_diff>
--- a/input_data.xlsx
+++ b/input_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johnp\code\GitHub\sailing_allocations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E60DB8CB-D9CD-4AA9-9C6A-6779AA15C928}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2AB6A77-0245-47CA-81F6-EA676E97B01D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1635" yWindow="3960" windowWidth="28800" windowHeight="11325" xr2:uid="{FB722AD1-E9B2-4C0B-A598-569FA88C88D2}"/>
+    <workbookView xWindow="1845" yWindow="1095" windowWidth="31980" windowHeight="12990" xr2:uid="{FB722AD1-E9B2-4C0B-A598-569FA88C88D2}"/>
   </bookViews>
   <sheets>
     <sheet name="Leader" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="Schedule" sheetId="5" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Leader!$A$1:$G$25</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Leader!$A$1:$H$25</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="108">
   <si>
     <t>Name</t>
   </si>
@@ -360,6 +360,9 @@
   </si>
   <si>
     <t>Cain M</t>
+  </si>
+  <si>
+    <t>CompRaceControl</t>
   </si>
 </sst>
 </file>
@@ -717,7 +720,7 @@
   <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -726,9 +729,9 @@
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" customWidth="1"/>
+    <col min="7" max="8" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -751,10 +754,10 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
+        <v>107</v>
+      </c>
+      <c r="H1" t="s">
         <v>34</v>
-      </c>
-      <c r="H1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -764,7 +767,7 @@
       <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="H2" t="s">
+      <c r="G2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -792,7 +795,7 @@
       <c r="F4" t="s">
         <v>8</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>15</v>
       </c>
     </row>
@@ -829,7 +832,7 @@
       <c r="F6" t="s">
         <v>8</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>15</v>
       </c>
     </row>
@@ -865,7 +868,7 @@
       <c r="F9" t="s">
         <v>8</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>15</v>
       </c>
     </row>
@@ -885,7 +888,7 @@
       <c r="F10" t="s">
         <v>8</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>15</v>
       </c>
     </row>
@@ -905,7 +908,7 @@
       <c r="F11" t="s">
         <v>8</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
         <v>15</v>
       </c>
     </row>
@@ -919,7 +922,7 @@
       <c r="E12" t="s">
         <v>8</v>
       </c>
-      <c r="G12" t="s">
+      <c r="H12" t="s">
         <v>16</v>
       </c>
     </row>
@@ -961,7 +964,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>62</v>
       </c>
@@ -969,7 +972,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>63</v>
       </c>
@@ -982,11 +985,11 @@
       <c r="F18" t="s">
         <v>8</v>
       </c>
-      <c r="G18" t="s">
+      <c r="H18" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>64</v>
       </c>
@@ -1000,7 +1003,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>65</v>
       </c>
@@ -1010,11 +1013,11 @@
       <c r="E20" t="s">
         <v>8</v>
       </c>
-      <c r="G20" t="s">
+      <c r="H20" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>66</v>
       </c>
@@ -1028,7 +1031,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>67</v>
       </c>
@@ -1039,7 +1042,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>68</v>
       </c>
@@ -1047,18 +1050,18 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>69</v>
       </c>
       <c r="B24" t="s">
         <v>9</v>
       </c>
-      <c r="G24" t="s">
+      <c r="H24" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>70</v>
       </c>
@@ -1073,7 +1076,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G25" xr:uid="{E855A98D-FCEC-4C7A-9164-30ACF8843399}"/>
+  <autoFilter ref="A1:H25" xr:uid="{E855A98D-FCEC-4C7A-9164-30ACF8843399}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>